<commit_message>
Image Scaling in Excel Export
</commit_message>
<xml_diff>
--- a/jxls-poi/src/test/resources/org/jxls/templatebasedtests/issue364Test.xlsx
+++ b/jxls-poi/src/test/resources/org/jxls/templatebasedtests/issue364Test.xlsx
@@ -51,7 +51,7 @@
             <charset val="0"/>
           </rPr>
           <t xml:space="preserve">
-jx:image(lastCell="C11" src="image" imageType="JPEG")</t>
+jx:image(lastCell="C11" src="image" imageType="JPEG" scaleX="1" scaleY="1")</t>
         </r>
       </text>
     </comment>
@@ -1216,7 +1216,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="3"/>

</xml_diff>